<commit_message>
Tratare exception, adnotari, mail etc
</commit_message>
<xml_diff>
--- a/rpaCrypto.xlsx
+++ b/rpaCrypto.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rpa" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
   <si>
     <t>Crypto Name</t>
   </si>
@@ -379,12 +379,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6 F6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -406,7 +406,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>29000</v>
+        <v>40000</v>
       </c>
       <c r="C2" s="1">
         <v>5</v>
@@ -436,11 +436,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -504,6 +506,126 @@
       </c>
       <c r="B8">
         <v>0.28160000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.31790000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>0.31380000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>38662.120000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>34713.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>34609.230000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0.29220000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>34257.21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>34286.879999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>34029.620000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>0.29060000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>34036.730000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>0.2913</v>
       </c>
     </row>
   </sheetData>
@@ -517,7 +639,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>